<commit_message>
refactor tests to that tests can be ran consecutively
</commit_message>
<xml_diff>
--- a/backend/src/__tests__/mock/StudentData.xlsx
+++ b/backend/src/__tests__/mock/StudentData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balqi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\user\School\DOP\Asgn 1\ias-2\backend\src\__tests__\mock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E515724-6069-4327-9FF8-74040A11F8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AB49C9-8E1B-4D56-9501-44D10C59915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="2000" windowWidth="14400" windowHeight="7870" xr2:uid="{5FE11085-A60F-4B7E-BD58-3D4972FE9776}"/>
+    <workbookView xWindow="1215" yWindow="225" windowWidth="21600" windowHeight="11385" xr2:uid="{5FE11085-A60F-4B7E-BD58-3D4972FE9776}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,27 +50,12 @@
     <t>Status</t>
   </si>
   <si>
-    <t>S12345678A</t>
-  </si>
-  <si>
-    <t>S12345678B</t>
-  </si>
-  <si>
-    <t>S12345678C</t>
-  </si>
-  <si>
-    <t>Balqis</t>
-  </si>
-  <si>
     <t>S12345678D</t>
   </si>
   <si>
     <t>Lala</t>
   </si>
   <si>
-    <t>Pooh</t>
-  </si>
-  <si>
     <t>Kinanti</t>
   </si>
   <si>
@@ -87,6 +72,21 @@
   </si>
   <si>
     <t>Unassigned</t>
+  </si>
+  <si>
+    <t>S12345670A</t>
+  </si>
+  <si>
+    <t>S12345671B</t>
+  </si>
+  <si>
+    <t>S12345677H</t>
+  </si>
+  <si>
+    <t>Student 8</t>
+  </si>
+  <si>
+    <t>Student 1</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,18 +441,18 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,60 +466,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>